<commit_message>
update burndown. add repos image. add 3.1.2, 3.1.4-7
</commit_message>
<xml_diff>
--- a/Formatted/burndown_sprint2.xlsx
+++ b/Formatted/burndown_sprint2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Dropbox\GimnasIO\Documentos\Informe_Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dari1\Documents\Github\GimnasIO-docs\Formatted\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16455" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16455" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="formulica" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>Fecha cierre</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Horas acumuladas</t>
   </si>
 </sst>
 </file>
@@ -2010,112 +2013,112 @@
                   <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>135</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>135</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>135</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>135</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>135</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>135</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>135</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>135</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>135</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>135</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>135</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>79</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>79</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>79</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -2314,112 +2317,112 @@
                   <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>135</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>135</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>135</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>135</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>135</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>135</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>135</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>135</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>135</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>135</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>135</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>135</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>79</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>79</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>79</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>32</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>0</c:v>
@@ -7069,23 +7072,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:L47"/>
+  <dimension ref="A5:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J47"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="67.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -7099,7 +7102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>43067</v>
       </c>
@@ -7129,7 +7132,7 @@
         <v>3.2142857142857144</v>
       </c>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>43068</v>
       </c>
@@ -7150,11 +7153,11 @@
         <v>119</v>
       </c>
       <c r="J7">
-        <f>SUM(J6+B7)</f>
+        <f>SUM(J6+A7)</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K47" si="1">135-J7</f>
+        <f t="shared" ref="K7:K18" si="1">135-J7</f>
         <v>135</v>
       </c>
       <c r="L7">
@@ -7162,7 +7165,7 @@
         <v>6.4285714285714288</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>43069</v>
       </c>
@@ -7183,7 +7186,7 @@
         <v>119</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J47" si="6">SUM(J7+B8)</f>
+        <f t="shared" ref="J8:J47" si="6">SUM(J7+A8)</f>
         <v>0</v>
       </c>
       <c r="K8">
@@ -7195,7 +7198,7 @@
         <v>9.6428571428571423</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>43070</v>
       </c>
@@ -7228,7 +7231,11 @@
         <v>12.857142857142858</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>(7+2+2)</f>
+        <v>11</v>
+      </c>
       <c r="E10" s="1">
         <v>43071</v>
       </c>
@@ -7250,18 +7257,18 @@
       </c>
       <c r="J10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
         <v>16.071428571428573</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>43072</v>
       </c>
@@ -7283,18 +7290,21 @@
       </c>
       <c r="J11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
         <v>19.285714285714288</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
       <c r="E12" s="1">
         <v>43073</v>
       </c>
@@ -7316,18 +7326,18 @@
       </c>
       <c r="J12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
         <v>22.500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <v>43074</v>
       </c>
@@ -7349,18 +7359,22 @@
       </c>
       <c r="J13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
         <v>25.714285714285719</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>2+16+2+3+3</f>
+        <v>26</v>
+      </c>
       <c r="E14" s="1">
         <v>43075</v>
       </c>
@@ -7382,18 +7396,22 @@
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
         <v>28.928571428571434</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>2+1+1+4</f>
+        <v>8</v>
+      </c>
       <c r="E15" s="1">
         <v>43076</v>
       </c>
@@ -7415,18 +7433,18 @@
       </c>
       <c r="J15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
         <v>32.142857142857146</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
         <v>43077</v>
       </c>
@@ -7448,18 +7466,22 @@
       </c>
       <c r="J16">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
         <v>35.357142857142861</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>1+1+4+2+6+4</f>
+        <v>18</v>
+      </c>
       <c r="E17" s="1">
         <v>43078</v>
       </c>
@@ -7481,18 +7503,18 @@
       </c>
       <c r="J17">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K17">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
         <v>38.571428571428577</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
         <v>43079</v>
       </c>
@@ -7514,18 +7536,18 @@
       </c>
       <c r="J18">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K18">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="L18">
         <f t="shared" si="2"/>
         <v>41.785714285714292</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E19" s="1">
         <v>43080</v>
       </c>
@@ -7547,18 +7569,18 @@
       </c>
       <c r="J19">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" ref="K7:K47" si="7">$A$48-J19</f>
+        <v>73</v>
       </c>
       <c r="L19">
         <f t="shared" si="2"/>
         <v>45.000000000000007</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E20" s="1">
         <v>43081</v>
       </c>
@@ -7580,18 +7602,18 @@
       </c>
       <c r="J20">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>73</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
         <v>48.214285714285722</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
         <v>43082</v>
       </c>
@@ -7613,18 +7635,18 @@
       </c>
       <c r="J21">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>73</v>
       </c>
       <c r="L21">
         <f t="shared" si="2"/>
         <v>51.428571428571438</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
         <v>43083</v>
       </c>
@@ -7646,18 +7668,18 @@
       </c>
       <c r="J22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>73</v>
       </c>
       <c r="L22">
         <f t="shared" si="2"/>
         <v>54.642857142857153</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
         <v>43084</v>
       </c>
@@ -7679,18 +7701,18 @@
       </c>
       <c r="J23">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>73</v>
       </c>
       <c r="L23">
         <f t="shared" si="2"/>
         <v>57.857142857142868</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
         <v>43085</v>
       </c>
@@ -7712,18 +7734,22 @@
       </c>
       <c r="J24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>73</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
         <v>61.071428571428584</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>3</f>
+        <v>3</v>
+      </c>
       <c r="E25" s="1">
         <v>43086</v>
       </c>
@@ -7745,18 +7771,22 @@
       </c>
       <c r="J25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>70</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
         <v>64.285714285714292</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>5+4+2+2+2+1</f>
+        <v>16</v>
+      </c>
       <c r="E26" s="1">
         <v>43087</v>
       </c>
@@ -7778,18 +7808,18 @@
       </c>
       <c r="J26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>54</v>
       </c>
       <c r="L26">
         <f t="shared" si="2"/>
         <v>67.5</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <v>43088</v>
       </c>
@@ -7811,18 +7841,22 @@
       </c>
       <c r="J27">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
-        <v>135</v>
+        <f t="shared" si="7"/>
+        <v>54</v>
       </c>
       <c r="L27">
         <f t="shared" si="2"/>
         <v>70.714285714285708</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>1+1+2+1</f>
+        <v>5</v>
+      </c>
       <c r="B28">
         <f>(13+4+9+10+19+1)</f>
         <v>56</v>
@@ -7855,18 +7889,18 @@
       </c>
       <c r="J28">
         <f t="shared" si="6"/>
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
-        <v>79</v>
+        <f t="shared" si="7"/>
+        <v>49</v>
       </c>
       <c r="L28">
         <f t="shared" si="2"/>
         <v>73.928571428571416</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E29" s="1">
         <v>43090</v>
       </c>
@@ -7888,18 +7922,18 @@
       </c>
       <c r="J29">
         <f t="shared" si="6"/>
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
-        <v>79</v>
+        <f t="shared" si="7"/>
+        <v>49</v>
       </c>
       <c r="L29">
         <f t="shared" si="2"/>
         <v>77.142857142857125</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E30" s="1">
         <v>43091</v>
       </c>
@@ -7921,18 +7955,22 @@
       </c>
       <c r="J30">
         <f t="shared" si="6"/>
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
-        <v>79</v>
+        <f t="shared" si="7"/>
+        <v>49</v>
       </c>
       <c r="L30">
         <f t="shared" si="2"/>
         <v>80.357142857142833</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>3+8+1+2+2+2+2+2</f>
+        <v>22</v>
+      </c>
       <c r="B31">
         <f>(11+3+5+3+6+6+4)</f>
         <v>38</v>
@@ -7965,23 +8003,23 @@
       </c>
       <c r="J31">
         <f t="shared" si="6"/>
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f t="shared" si="7"/>
+        <v>27</v>
       </c>
       <c r="L31">
         <f t="shared" si="2"/>
         <v>83.571428571428541</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E32" s="1">
         <v>43093</v>
       </c>
       <c r="F32">
-        <f t="shared" ref="F32:F47" si="7">SUM(F31+C32)</f>
+        <f t="shared" ref="F32:F47" si="8">SUM(F31+C32)</f>
         <v>83</v>
       </c>
       <c r="G32">
@@ -7998,23 +8036,23 @@
       </c>
       <c r="J32">
         <f t="shared" si="6"/>
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f t="shared" si="7"/>
+        <v>27</v>
       </c>
       <c r="L32">
         <f t="shared" si="2"/>
         <v>86.785714285714249</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E33" s="1">
         <v>43094</v>
       </c>
       <c r="F33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="G33">
@@ -8031,23 +8069,23 @@
       </c>
       <c r="J33">
         <f t="shared" si="6"/>
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f t="shared" si="7"/>
+        <v>27</v>
       </c>
       <c r="L33">
         <f t="shared" si="2"/>
         <v>89.999999999999957</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E34" s="1">
         <v>43095</v>
       </c>
       <c r="F34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="G34">
@@ -8064,18 +8102,21 @@
       </c>
       <c r="J34">
         <f t="shared" si="6"/>
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f t="shared" si="7"/>
+        <v>27</v>
       </c>
       <c r="L34">
         <f t="shared" si="2"/>
         <v>93.214285714285666</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
       <c r="B35">
         <v>9</v>
       </c>
@@ -8089,7 +8130,7 @@
         <v>43096</v>
       </c>
       <c r="F35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>91</v>
       </c>
       <c r="G35">
@@ -8106,23 +8147,23 @@
       </c>
       <c r="J35">
         <f t="shared" si="6"/>
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f t="shared" si="7"/>
+        <v>23</v>
       </c>
       <c r="L35">
         <f t="shared" si="2"/>
         <v>96.428571428571374</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E36" s="1">
         <v>43097</v>
       </c>
       <c r="F36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>91</v>
       </c>
       <c r="G36">
@@ -8139,23 +8180,23 @@
       </c>
       <c r="J36">
         <f t="shared" si="6"/>
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="K36">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f t="shared" si="7"/>
+        <v>23</v>
       </c>
       <c r="L36">
         <f t="shared" si="2"/>
         <v>99.642857142857082</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E37" s="1">
         <v>43098</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>91</v>
       </c>
       <c r="G37">
@@ -8172,23 +8213,23 @@
       </c>
       <c r="J37">
         <f t="shared" si="6"/>
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="K37">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f t="shared" si="7"/>
+        <v>23</v>
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
         <v>102.85714285714279</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E38" s="1">
         <v>43099</v>
       </c>
       <c r="F38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>91</v>
       </c>
       <c r="G38">
@@ -8205,18 +8246,22 @@
       </c>
       <c r="J38">
         <f t="shared" si="6"/>
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="K38">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f t="shared" si="7"/>
+        <v>23</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
         <v>106.0714285714285</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>8+2+3</f>
+        <v>13</v>
+      </c>
       <c r="B39">
         <v>13</v>
       </c>
@@ -8230,7 +8275,7 @@
         <v>43100</v>
       </c>
       <c r="F39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G39">
@@ -8247,23 +8292,23 @@
       </c>
       <c r="J39">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K39">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
         <v>109.28571428571421</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E40" s="1">
         <v>43101</v>
       </c>
       <c r="F40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G40">
@@ -8280,23 +8325,23 @@
       </c>
       <c r="J40">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K40">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
         <v>112.49999999999991</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E41" s="1">
         <v>43102</v>
       </c>
       <c r="F41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G41">
@@ -8313,23 +8358,23 @@
       </c>
       <c r="J41">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K41">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
         <v>115.71428571428562</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E42" s="1">
         <v>43103</v>
       </c>
       <c r="F42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G42">
@@ -8346,23 +8391,23 @@
       </c>
       <c r="J42">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K42">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
         <v>118.92857142857133</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E43" s="1">
         <v>43104</v>
       </c>
       <c r="F43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G43">
@@ -8379,23 +8424,23 @@
       </c>
       <c r="J43">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K43">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
         <v>122.14285714285704</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E44" s="1">
         <v>43105</v>
       </c>
       <c r="F44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G44">
@@ -8412,23 +8457,23 @@
       </c>
       <c r="J44">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K44">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
         <v>125.35714285714275</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E45" s="1">
         <v>43106</v>
       </c>
       <c r="F45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>99</v>
       </c>
       <c r="G45">
@@ -8445,18 +8490,22 @@
       </c>
       <c r="J45">
         <f t="shared" si="6"/>
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K45">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
         <v>128.57142857142847</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f>3+6+1</f>
+        <v>10</v>
+      </c>
       <c r="B46">
         <v>19</v>
       </c>
@@ -8470,7 +8519,7 @@
         <v>43107</v>
       </c>
       <c r="F46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>119</v>
       </c>
       <c r="G46">
@@ -8487,10 +8536,10 @@
       </c>
       <c r="J46">
         <f t="shared" si="6"/>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L46">
@@ -8498,12 +8547,12 @@
         <v>131.78571428571419</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E47" s="1">
         <v>43108</v>
       </c>
       <c r="F47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>119</v>
       </c>
       <c r="G47">
@@ -8520,15 +8569,21 @@
       </c>
       <c r="J47">
         <f t="shared" si="6"/>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
         <v>134.99999999999991</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f>SUM(A6:A46)</f>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -9112,8 +9167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9129,7 +9184,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -9208,10 +9263,10 @@
         <v>125.35714285714275</v>
       </c>
       <c r="E6">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F6">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -9225,10 +9280,10 @@
         <v>122.14285714285704</v>
       </c>
       <c r="E7">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F7">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -9242,10 +9297,10 @@
         <v>118.92857142857133</v>
       </c>
       <c r="E8">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F8">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -9259,10 +9314,10 @@
         <v>115.71428571428562</v>
       </c>
       <c r="E9">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F9">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -9276,10 +9331,10 @@
         <v>112.49999999999991</v>
       </c>
       <c r="E10">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="F10">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -9293,10 +9348,10 @@
         <v>109.28571428571421</v>
       </c>
       <c r="E11">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="F11">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -9310,10 +9365,10 @@
         <v>106.0714285714285</v>
       </c>
       <c r="E12">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="F12">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -9327,10 +9382,10 @@
         <v>102.85714285714279</v>
       </c>
       <c r="E13">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="F13">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -9350,10 +9405,10 @@
         <v>99.642857142857082</v>
       </c>
       <c r="E14">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="F14">
-        <v>135</v>
+        <v>71</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -9367,10 +9422,10 @@
         <v>96.428571428571374</v>
       </c>
       <c r="E15">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F15">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -9384,10 +9439,10 @@
         <v>93.214285714285666</v>
       </c>
       <c r="E16">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F16">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -9401,10 +9456,10 @@
         <v>89.999999999999957</v>
       </c>
       <c r="E17">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F17">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -9418,10 +9473,10 @@
         <v>86.785714285714249</v>
       </c>
       <c r="E18">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F18">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -9435,10 +9490,10 @@
         <v>83.571428571428541</v>
       </c>
       <c r="E19">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F19">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -9452,10 +9507,10 @@
         <v>80.357142857142833</v>
       </c>
       <c r="E20">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F20">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -9475,10 +9530,10 @@
         <v>77.142857142857125</v>
       </c>
       <c r="E21">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="F21">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -9498,10 +9553,10 @@
         <v>73.928571428571416</v>
       </c>
       <c r="E22">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="F22">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -9515,10 +9570,10 @@
         <v>70.714285714285708</v>
       </c>
       <c r="E23">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="F23">
-        <v>135</v>
+        <v>54</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -9532,10 +9587,10 @@
         <v>67.5</v>
       </c>
       <c r="E24">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F24">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="G24">
         <v>56</v>
@@ -9549,10 +9604,10 @@
         <v>64.285714285714292</v>
       </c>
       <c r="E25">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F25">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="G25">
         <v>56</v>
@@ -9572,10 +9627,10 @@
         <v>61.071428571428584</v>
       </c>
       <c r="E26">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="F26">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="G26">
         <v>56</v>
@@ -9595,10 +9650,10 @@
         <v>57.857142857142868</v>
       </c>
       <c r="E27">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F27">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G27">
         <v>94</v>
@@ -9612,10 +9667,10 @@
         <v>54.642857142857153</v>
       </c>
       <c r="E28">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F28">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G28">
         <v>94</v>
@@ -9629,10 +9684,10 @@
         <v>51.428571428571438</v>
       </c>
       <c r="E29">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F29">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G29">
         <v>94</v>
@@ -9646,10 +9701,10 @@
         <v>48.214285714285722</v>
       </c>
       <c r="E30">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F30">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G30">
         <v>94</v>
@@ -9663,10 +9718,10 @@
         <v>45.000000000000007</v>
       </c>
       <c r="E31">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F31">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G31">
         <v>103</v>
@@ -9680,10 +9735,10 @@
         <v>41.785714285714292</v>
       </c>
       <c r="E32">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F32">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G32">
         <v>103</v>
@@ -9697,10 +9752,10 @@
         <v>38.571428571428577</v>
       </c>
       <c r="E33">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F33">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G33">
         <v>103</v>
@@ -9714,10 +9769,10 @@
         <v>35.357142857142861</v>
       </c>
       <c r="E34">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F34">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G34">
         <v>103</v>
@@ -9731,10 +9786,10 @@
         <v>32.142857142857146</v>
       </c>
       <c r="E35">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F35">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G35">
         <v>116</v>
@@ -9748,10 +9803,10 @@
         <v>28.928571428571434</v>
       </c>
       <c r="E36">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F36">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>116</v>
@@ -9765,10 +9820,10 @@
         <v>25.714285714285719</v>
       </c>
       <c r="E37">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F37">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G37">
         <v>116</v>
@@ -9782,10 +9837,10 @@
         <v>22.500000000000004</v>
       </c>
       <c r="E38">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F38">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G38">
         <v>116</v>
@@ -9799,10 +9854,10 @@
         <v>19.285714285714288</v>
       </c>
       <c r="E39">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F39">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G39">
         <v>116</v>
@@ -9816,10 +9871,10 @@
         <v>16.071428571428573</v>
       </c>
       <c r="E40">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F40">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G40">
         <v>116</v>
@@ -9833,10 +9888,10 @@
         <v>12.857142857142858</v>
       </c>
       <c r="E41">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F41">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G41">
         <v>116</v>
@@ -9856,7 +9911,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
@@ -9873,7 +9928,7 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
@@ -9890,7 +9945,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>134.87224157955799</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -9906,7 +9961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
@@ -10680,7 +10735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223A9E8A-A352-4DA8-B25A-0D0B9ED00691}">
   <dimension ref="E5:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>

</xml_diff>